<commit_message>
Added table with selected project data
</commit_message>
<xml_diff>
--- a/final-confirmed_2022_6_23 - kopie.xlsx
+++ b/final-confirmed_2022_6_23 - kopie.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\MIMRNAK\Python\automatizace_odb\exporty_odb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/095fcb64233a8419/Dokumenty/pythonProject/database_automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_A24293CB86A3F32D4B4A2B04C4337BC68D962928" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7BB669F-822E-4C36-B8A7-3E63F897992A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="75" yWindow="3120" windowWidth="25440" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAD" sheetId="1" r:id="rId1"/>
@@ -21,12 +22,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="M6" authorId="0" shapeId="0">
+    <comment ref="M6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -42,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N6" authorId="0" shapeId="0">
+    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L7" authorId="0" shapeId="0">
+    <comment ref="L7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -75,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M7" authorId="0" shapeId="0">
+    <comment ref="M7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -92,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0" shapeId="0">
+    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M8" authorId="0" shapeId="0">
+    <comment ref="M8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -126,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0" shapeId="0">
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -143,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L9" authorId="0" shapeId="0">
+    <comment ref="L9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -160,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M9" authorId="0" shapeId="0">
+    <comment ref="M9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -177,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N9" authorId="0" shapeId="0">
+    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -375,7 +376,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
@@ -433,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -441,9 +442,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -742,7 +744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -756,6 +758,7 @@
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -1221,8 +1224,8 @@
         <v>6.25</v>
       </c>
       <c r="O9" s="2"/>
-      <c r="P9" s="2">
-        <v>250</v>
+      <c r="P9" s="7">
+        <v>44743</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2">
@@ -1251,7 +1254,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1417,7 +1420,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated and improved gui. Added value of used hours previous month.
</commit_message>
<xml_diff>
--- a/final-confirmed_2022_6_23 - kopie.xlsx
+++ b/final-confirmed_2022_6_23 - kopie.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/095fcb64233a8419/Dokumenty/pythonProject/database_automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_A24293CB86A3F32D4B4A2B04C4337BC68D962928" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7BB669F-822E-4C36-B8A7-3E63F897992A}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_A24293CB86A3F32D4B4A2B04C4337BC68D962928" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7C8A2A3-7A35-4D6A-9A4D-B67519531B13}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="3120" windowWidth="25440" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="1800" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAD" sheetId="1" r:id="rId1"/>
     <sheet name="FEM" sheetId="2" r:id="rId2"/>
     <sheet name="CFD" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -747,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>